<commit_message>
added visualizations, added records
</commit_message>
<xml_diff>
--- a/data/corona_cases_ksa.xlsx
+++ b/data/corona_cases_ksa.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mohammedalawami/Desktop/Learn Data Science/Projects/corona-data-challenge/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15AF470D-D191-A641-A9DB-AAC048DE8ECA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81552D6A-5904-064E-ABF2-C20278065F28}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1120" yWindow="460" windowWidth="33600" windowHeight="19260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="33600" windowHeight="20640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="71">
   <si>
     <t>date</t>
   </si>
@@ -228,6 +228,21 @@
   </si>
   <si>
     <t>Abha</t>
+  </si>
+  <si>
+    <t>Afghanistan</t>
+  </si>
+  <si>
+    <t>Arar</t>
+  </si>
+  <si>
+    <t>Jubail</t>
+  </si>
+  <si>
+    <t>Al Hudud ash Shamaliyah</t>
+  </si>
+  <si>
+    <t>Northern Frontier</t>
   </si>
 </sst>
 </file>
@@ -237,7 +252,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -249,6 +264,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -289,12 +311,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -633,15 +657,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H149"/>
+  <dimension ref="A1:N158"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="A140" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="E162" sqref="E162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
@@ -2286,6 +2311,9 @@
       <c r="E64">
         <v>1</v>
       </c>
+      <c r="F64" t="s">
+        <v>66</v>
+      </c>
       <c r="G64" t="s">
         <v>57</v>
       </c>
@@ -2293,7 +2321,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A65" s="2">
         <v>43907</v>
       </c>
@@ -2319,7 +2347,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A66" s="2">
         <v>43907</v>
       </c>
@@ -2345,7 +2373,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A67" s="2">
         <v>43907</v>
       </c>
@@ -2370,8 +2398,9 @@
       <c r="H67" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="M67" s="3"/>
+    </row>
+    <row r="68" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A68" s="2">
         <v>43907</v>
       </c>
@@ -2396,8 +2425,9 @@
       <c r="H68" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="M68" s="3"/>
+    </row>
+    <row r="69" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A69" s="2">
         <v>43907</v>
       </c>
@@ -2422,8 +2452,10 @@
       <c r="H69" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="M69" s="3"/>
+      <c r="N69" s="4"/>
+    </row>
+    <row r="70" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A70" s="2">
         <v>43907</v>
       </c>
@@ -2448,8 +2480,9 @@
       <c r="H70" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="M70" s="3"/>
+    </row>
+    <row r="71" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A71" s="2">
         <v>43907</v>
       </c>
@@ -2474,8 +2507,9 @@
       <c r="H71" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="M71" s="3"/>
+    </row>
+    <row r="72" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A72" s="2">
         <v>43907</v>
       </c>
@@ -2500,8 +2534,9 @@
       <c r="H72" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="M72" s="3"/>
+    </row>
+    <row r="73" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A73" s="2">
         <v>43907</v>
       </c>
@@ -2523,8 +2558,9 @@
       <c r="H73" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="M73" s="3"/>
+    </row>
+    <row r="74" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A74" s="2">
         <v>43907</v>
       </c>
@@ -2549,8 +2585,9 @@
       <c r="H74" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="M74" s="3"/>
+    </row>
+    <row r="75" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A75" s="2">
         <v>43907</v>
       </c>
@@ -2575,8 +2612,9 @@
       <c r="H75" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="M75" s="3"/>
+    </row>
+    <row r="76" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A76" s="2">
         <v>43907</v>
       </c>
@@ -2601,8 +2639,9 @@
       <c r="H76" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="M76" s="3"/>
+    </row>
+    <row r="77" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A77" s="2">
         <v>43907</v>
       </c>
@@ -2627,8 +2666,9 @@
       <c r="H77" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="M77" s="3"/>
+    </row>
+    <row r="78" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A78" s="2">
         <v>43907</v>
       </c>
@@ -2653,8 +2693,9 @@
       <c r="H78" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="M78" s="3"/>
+    </row>
+    <row r="79" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A79" s="2">
         <v>43907</v>
       </c>
@@ -2679,8 +2720,9 @@
       <c r="H79" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="M79" s="3"/>
+    </row>
+    <row r="80" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A80" s="2">
         <v>43907</v>
       </c>
@@ -2705,8 +2747,9 @@
       <c r="H80" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="M80" s="3"/>
+    </row>
+    <row r="81" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A81" s="2">
         <v>43907</v>
       </c>
@@ -2731,8 +2774,9 @@
       <c r="H81" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="M81" s="3"/>
+    </row>
+    <row r="82" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A82" s="2">
         <v>43907</v>
       </c>
@@ -2757,8 +2801,9 @@
       <c r="H82" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="M82" s="3"/>
+    </row>
+    <row r="83" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A83" s="2">
         <v>43907</v>
       </c>
@@ -2783,8 +2828,9 @@
       <c r="H83" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="M83" s="3"/>
+    </row>
+    <row r="84" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A84" s="2">
         <v>43907</v>
       </c>
@@ -2809,8 +2855,9 @@
       <c r="H84" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="M84" s="3"/>
+    </row>
+    <row r="85" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A85" s="2">
         <v>43907</v>
       </c>
@@ -2835,8 +2882,9 @@
       <c r="H85" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="M85" s="3"/>
+    </row>
+    <row r="86" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A86" s="2">
         <v>43907</v>
       </c>
@@ -2852,8 +2900,9 @@
       <c r="H86" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="M86" s="3"/>
+    </row>
+    <row r="87" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A87" s="2">
         <v>43908</v>
       </c>
@@ -2872,8 +2921,9 @@
       <c r="H87" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="M87" s="3"/>
+    </row>
+    <row r="88" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A88" s="2">
         <v>43908</v>
       </c>
@@ -2889,8 +2939,9 @@
       <c r="H88" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="M88" s="3"/>
+    </row>
+    <row r="89" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A89" s="2">
         <v>43908</v>
       </c>
@@ -2909,8 +2960,9 @@
       <c r="H89" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="M89" s="3"/>
+    </row>
+    <row r="90" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A90" s="2">
         <v>43908</v>
       </c>
@@ -2927,7 +2979,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A91" s="2">
         <v>43908</v>
       </c>
@@ -2947,7 +2999,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A92" s="2">
         <v>43909</v>
       </c>
@@ -2967,7 +3019,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A93" s="2">
         <v>43909</v>
       </c>
@@ -2987,7 +3039,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A94" s="2">
         <v>43909</v>
       </c>
@@ -3007,7 +3059,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A95" s="2">
         <v>43909</v>
       </c>
@@ -3027,7 +3079,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A96" s="2">
         <v>43909</v>
       </c>
@@ -3862,7 +3914,7 @@
         <v>9</v>
       </c>
       <c r="D137">
-        <f t="shared" ref="D137:D147" si="0" xml:space="preserve"> D136+E137</f>
+        <f t="shared" ref="D137:D158" si="0" xml:space="preserve"> D136+E137</f>
         <v>713</v>
       </c>
       <c r="E137">
@@ -4083,10 +4135,235 @@
       </c>
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A148" s="2"/>
+      <c r="A148" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B148" t="s">
+        <v>9</v>
+      </c>
+      <c r="C148" t="s">
+        <v>9</v>
+      </c>
+      <c r="D148">
+        <f t="shared" si="0"/>
+        <v>850</v>
+      </c>
+      <c r="E148">
+        <v>83</v>
+      </c>
+      <c r="H148" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A149" s="2"/>
+      <c r="A149" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B149" t="s">
+        <v>15</v>
+      </c>
+      <c r="C149" t="s">
+        <v>28</v>
+      </c>
+      <c r="D149">
+        <f t="shared" si="0"/>
+        <v>863</v>
+      </c>
+      <c r="E149">
+        <v>13</v>
+      </c>
+      <c r="H149" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="150" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A150" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B150" t="s">
+        <v>11</v>
+      </c>
+      <c r="C150" t="s">
+        <v>29</v>
+      </c>
+      <c r="D150">
+        <f t="shared" si="0"/>
+        <v>873</v>
+      </c>
+      <c r="E150">
+        <v>10</v>
+      </c>
+      <c r="H150" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="151" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A151" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B151" t="s">
+        <v>18</v>
+      </c>
+      <c r="C151" t="s">
+        <v>18</v>
+      </c>
+      <c r="D151">
+        <f t="shared" si="0"/>
+        <v>879</v>
+      </c>
+      <c r="E151">
+        <v>6</v>
+      </c>
+      <c r="H151" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="152" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A152" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B152" t="s">
+        <v>8</v>
+      </c>
+      <c r="C152" t="s">
+        <v>28</v>
+      </c>
+      <c r="D152">
+        <f t="shared" si="0"/>
+        <v>885</v>
+      </c>
+      <c r="E152">
+        <v>6</v>
+      </c>
+      <c r="H152" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="153" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A153" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B153" t="s">
+        <v>13</v>
+      </c>
+      <c r="C153" t="s">
+        <v>28</v>
+      </c>
+      <c r="D153">
+        <f t="shared" si="0"/>
+        <v>890</v>
+      </c>
+      <c r="E153">
+        <v>5</v>
+      </c>
+      <c r="H153" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="154" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A154" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B154" t="s">
+        <v>26</v>
+      </c>
+      <c r="C154" t="s">
+        <v>26</v>
+      </c>
+      <c r="D154">
+        <f t="shared" si="0"/>
+        <v>894</v>
+      </c>
+      <c r="E154">
+        <v>4</v>
+      </c>
+      <c r="H154" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="155" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A155" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B155" t="s">
+        <v>65</v>
+      </c>
+      <c r="C155" t="s">
+        <v>30</v>
+      </c>
+      <c r="D155">
+        <f t="shared" si="0"/>
+        <v>896</v>
+      </c>
+      <c r="E155">
+        <v>2</v>
+      </c>
+      <c r="H155" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="156" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A156" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B156" t="s">
+        <v>67</v>
+      </c>
+      <c r="C156" t="s">
+        <v>70</v>
+      </c>
+      <c r="D156">
+        <f t="shared" si="0"/>
+        <v>898</v>
+      </c>
+      <c r="E156">
+        <v>2</v>
+      </c>
+      <c r="H156" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="157" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A157" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B157" t="s">
+        <v>14</v>
+      </c>
+      <c r="C157" t="s">
+        <v>28</v>
+      </c>
+      <c r="D157">
+        <f t="shared" si="0"/>
+        <v>899</v>
+      </c>
+      <c r="E157">
+        <v>1</v>
+      </c>
+      <c r="H157" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="158" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A158" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B158" t="s">
+        <v>68</v>
+      </c>
+      <c r="C158" t="s">
+        <v>28</v>
+      </c>
+      <c r="D158">
+        <f t="shared" si="0"/>
+        <v>900</v>
+      </c>
+      <c r="E158">
+        <v>1</v>
+      </c>
+      <c r="H158" t="s">
+        <v>59</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added visualizations, updated dataset, added another map plot
</commit_message>
<xml_diff>
--- a/data/corona_cases_ksa.xlsx
+++ b/data/corona_cases_ksa.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mohammedalawami/Desktop/Learn Data Science/Projects/corona-data-challenge/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81552D6A-5904-064E-ABF2-C20278065F28}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E7F79AB-CE32-3347-BBD5-CA719069A9C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="33600" windowHeight="20640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="73">
   <si>
     <t>date</t>
   </si>
@@ -243,6 +243,12 @@
   </si>
   <si>
     <t>Northern Frontier</t>
+  </si>
+  <si>
+    <t>Buraidah</t>
+  </si>
+  <si>
+    <t>Khafji</t>
   </si>
 </sst>
 </file>
@@ -657,10 +663,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N158"/>
+  <dimension ref="A1:N170"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A140" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E162" sqref="E162"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="G75" sqref="G75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2888,6 +2894,9 @@
       <c r="A86" s="2">
         <v>43907</v>
       </c>
+      <c r="B86" t="s">
+        <v>9</v>
+      </c>
       <c r="C86" t="s">
         <v>9</v>
       </c>
@@ -3914,7 +3923,7 @@
         <v>9</v>
       </c>
       <c r="D137">
-        <f t="shared" ref="D137:D158" si="0" xml:space="preserve"> D136+E137</f>
+        <f t="shared" ref="D137:D170" si="0" xml:space="preserve"> D136+E137</f>
         <v>713</v>
       </c>
       <c r="E137">
@@ -4362,6 +4371,258 @@
         <v>1</v>
       </c>
       <c r="H158" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="159" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A159" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B159" t="s">
+        <v>9</v>
+      </c>
+      <c r="C159" t="s">
+        <v>9</v>
+      </c>
+      <c r="D159">
+        <f t="shared" si="0"/>
+        <v>934</v>
+      </c>
+      <c r="E159">
+        <v>34</v>
+      </c>
+      <c r="H159" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="160" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A160" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B160" t="s">
+        <v>10</v>
+      </c>
+      <c r="C160" t="s">
+        <v>29</v>
+      </c>
+      <c r="D160">
+        <f t="shared" si="0"/>
+        <v>960</v>
+      </c>
+      <c r="E160">
+        <v>26</v>
+      </c>
+      <c r="H160" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="161" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A161" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B161" t="s">
+        <v>25</v>
+      </c>
+      <c r="C161" t="s">
+        <v>29</v>
+      </c>
+      <c r="D161">
+        <f t="shared" si="0"/>
+        <v>978</v>
+      </c>
+      <c r="E161">
+        <v>18</v>
+      </c>
+      <c r="H161" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="162" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A162" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B162" t="s">
+        <v>11</v>
+      </c>
+      <c r="C162" t="s">
+        <v>29</v>
+      </c>
+      <c r="D162">
+        <f t="shared" si="0"/>
+        <v>991</v>
+      </c>
+      <c r="E162">
+        <v>13</v>
+      </c>
+      <c r="H162" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="163" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A163" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B163" t="s">
+        <v>15</v>
+      </c>
+      <c r="C163" t="s">
+        <v>28</v>
+      </c>
+      <c r="D163">
+        <f t="shared" si="0"/>
+        <v>997</v>
+      </c>
+      <c r="E163">
+        <v>6</v>
+      </c>
+      <c r="H163" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="164" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A164" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B164" t="s">
+        <v>8</v>
+      </c>
+      <c r="C164" t="s">
+        <v>28</v>
+      </c>
+      <c r="D164">
+        <f t="shared" si="0"/>
+        <v>1002</v>
+      </c>
+      <c r="E164">
+        <v>5</v>
+      </c>
+      <c r="H164" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="165" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A165" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B165" t="s">
+        <v>18</v>
+      </c>
+      <c r="C165" t="s">
+        <v>18</v>
+      </c>
+      <c r="D165">
+        <f t="shared" si="0"/>
+        <v>1005</v>
+      </c>
+      <c r="E165">
+        <v>3</v>
+      </c>
+      <c r="H165" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="166" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A166" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B166" t="s">
+        <v>13</v>
+      </c>
+      <c r="C166" t="s">
+        <v>28</v>
+      </c>
+      <c r="D166">
+        <f t="shared" si="0"/>
+        <v>1007</v>
+      </c>
+      <c r="E166">
+        <v>2</v>
+      </c>
+      <c r="H166" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="167" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A167" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B167" t="s">
+        <v>12</v>
+      </c>
+      <c r="C167" t="s">
+        <v>28</v>
+      </c>
+      <c r="D167">
+        <f t="shared" si="0"/>
+        <v>1009</v>
+      </c>
+      <c r="E167">
+        <v>2</v>
+      </c>
+      <c r="H167" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="168" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A168" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B168" t="s">
+        <v>14</v>
+      </c>
+      <c r="C168" t="s">
+        <v>28</v>
+      </c>
+      <c r="D168">
+        <f t="shared" si="0"/>
+        <v>1010</v>
+      </c>
+      <c r="E168">
+        <v>1</v>
+      </c>
+      <c r="H168" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="169" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A169" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B169" t="s">
+        <v>71</v>
+      </c>
+      <c r="C169" t="s">
+        <v>32</v>
+      </c>
+      <c r="D169">
+        <f t="shared" si="0"/>
+        <v>1011</v>
+      </c>
+      <c r="E169">
+        <v>1</v>
+      </c>
+      <c r="H169" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="170" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A170" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B170" t="s">
+        <v>72</v>
+      </c>
+      <c r="C170" t="s">
+        <v>28</v>
+      </c>
+      <c r="D170">
+        <f t="shared" si="0"/>
+        <v>1012</v>
+      </c>
+      <c r="E170">
+        <v>1</v>
+      </c>
+      <c r="H170" t="s">
         <v>59</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added visualizations, updated ksa dataset
</commit_message>
<xml_diff>
--- a/data/corona_cases_ksa.xlsx
+++ b/data/corona_cases_ksa.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mohammedalawami/Desktop/Learn Data Science/Projects/corona-data-challenge/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E7F79AB-CE32-3347-BBD5-CA719069A9C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC9AD0C1-3363-1D44-AEFE-16A339AEB28F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="33600" windowHeight="20640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="704" uniqueCount="73">
   <si>
     <t>date</t>
   </si>
@@ -663,10 +663,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N170"/>
+  <dimension ref="A1:N179"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="G75" sqref="G75"/>
+    <sheetView tabSelected="1" topLeftCell="A151" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="H180" sqref="H180"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3923,7 +3923,7 @@
         <v>9</v>
       </c>
       <c r="D137">
-        <f t="shared" ref="D137:D170" si="0" xml:space="preserve"> D136+E137</f>
+        <f t="shared" ref="D137:D179" si="0" xml:space="preserve"> D136+E137</f>
         <v>713</v>
       </c>
       <c r="E137">
@@ -4623,6 +4623,195 @@
         <v>1</v>
       </c>
       <c r="H170" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="171" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A171" s="2">
+        <v>43917</v>
+      </c>
+      <c r="B171" t="s">
+        <v>9</v>
+      </c>
+      <c r="C171" t="s">
+        <v>9</v>
+      </c>
+      <c r="D171">
+        <f t="shared" si="0"/>
+        <v>1058</v>
+      </c>
+      <c r="E171">
+        <v>46</v>
+      </c>
+      <c r="H171" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="172" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A172" s="2">
+        <v>43917</v>
+      </c>
+      <c r="B172" t="s">
+        <v>18</v>
+      </c>
+      <c r="C172" t="s">
+        <v>18</v>
+      </c>
+      <c r="D172">
+        <f t="shared" si="0"/>
+        <v>1077</v>
+      </c>
+      <c r="E172">
+        <v>19</v>
+      </c>
+      <c r="H172" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="173" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A173" s="2">
+        <v>43917</v>
+      </c>
+      <c r="B173" t="s">
+        <v>8</v>
+      </c>
+      <c r="C173" t="s">
+        <v>28</v>
+      </c>
+      <c r="D173">
+        <f t="shared" si="0"/>
+        <v>1087</v>
+      </c>
+      <c r="E173">
+        <v>10</v>
+      </c>
+      <c r="H173" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="174" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A174" s="2">
+        <v>43917</v>
+      </c>
+      <c r="B174" t="s">
+        <v>11</v>
+      </c>
+      <c r="C174" t="s">
+        <v>29</v>
+      </c>
+      <c r="D174">
+        <f t="shared" si="0"/>
+        <v>1094</v>
+      </c>
+      <c r="E174">
+        <v>7</v>
+      </c>
+      <c r="H174" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="175" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A175" s="2">
+        <v>43917</v>
+      </c>
+      <c r="B175" t="s">
+        <v>15</v>
+      </c>
+      <c r="C175" t="s">
+        <v>28</v>
+      </c>
+      <c r="D175">
+        <f t="shared" si="0"/>
+        <v>1098</v>
+      </c>
+      <c r="E175">
+        <v>4</v>
+      </c>
+      <c r="H175" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="176" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A176" s="2">
+        <v>43917</v>
+      </c>
+      <c r="B176" t="s">
+        <v>14</v>
+      </c>
+      <c r="C176" t="s">
+        <v>28</v>
+      </c>
+      <c r="D176">
+        <f t="shared" si="0"/>
+        <v>1100</v>
+      </c>
+      <c r="E176">
+        <v>2</v>
+      </c>
+      <c r="H176" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="177" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A177" s="2">
+        <v>43917</v>
+      </c>
+      <c r="B177" t="s">
+        <v>71</v>
+      </c>
+      <c r="C177" t="s">
+        <v>32</v>
+      </c>
+      <c r="D177">
+        <f t="shared" si="0"/>
+        <v>1102</v>
+      </c>
+      <c r="E177">
+        <v>2</v>
+      </c>
+      <c r="H177" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="178" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A178" s="2">
+        <v>43917</v>
+      </c>
+      <c r="B178" t="s">
+        <v>12</v>
+      </c>
+      <c r="C178" t="s">
+        <v>28</v>
+      </c>
+      <c r="D178">
+        <f t="shared" si="0"/>
+        <v>1103</v>
+      </c>
+      <c r="E178">
+        <v>1</v>
+      </c>
+      <c r="H178" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="179" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A179" s="2">
+        <v>43917</v>
+      </c>
+      <c r="B179" t="s">
+        <v>13</v>
+      </c>
+      <c r="C179" t="s">
+        <v>28</v>
+      </c>
+      <c r="D179">
+        <f t="shared" si="0"/>
+        <v>1104</v>
+      </c>
+      <c r="E179">
+        <v>1</v>
+      </c>
+      <c r="H179" t="s">
         <v>59</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated dataset, added prediction model
</commit_message>
<xml_diff>
--- a/data/corona_cases_ksa.xlsx
+++ b/data/corona_cases_ksa.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mohammedalawami/Desktop/Learn Data Science/Projects/corona-data-challenge/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC9AD0C1-3363-1D44-AEFE-16A339AEB28F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62CEB2B6-07F9-1346-BFD6-26D65AB96BC5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="33600" windowHeight="20640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="704" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="737" uniqueCount="74">
   <si>
     <t>date</t>
   </si>
@@ -249,6 +249,9 @@
   </si>
   <si>
     <t>Khafji</t>
+  </si>
+  <si>
+    <t>Khamis Mushait</t>
   </si>
 </sst>
 </file>
@@ -663,10 +666,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N179"/>
+  <dimension ref="A1:N190"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A151" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="H180" sqref="H180"/>
+    <sheetView tabSelected="1" topLeftCell="A159" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="G192" sqref="G192"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3923,7 +3926,7 @@
         <v>9</v>
       </c>
       <c r="D137">
-        <f t="shared" ref="D137:D179" si="0" xml:space="preserve"> D136+E137</f>
+        <f t="shared" ref="D137:D190" si="0" xml:space="preserve"> D136+E137</f>
         <v>713</v>
       </c>
       <c r="E137">
@@ -4812,6 +4815,237 @@
         <v>1</v>
       </c>
       <c r="H179" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="180" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A180" s="2">
+        <v>43918</v>
+      </c>
+      <c r="B180" t="s">
+        <v>9</v>
+      </c>
+      <c r="C180" t="s">
+        <v>9</v>
+      </c>
+      <c r="D180">
+        <f t="shared" si="0"/>
+        <v>1145</v>
+      </c>
+      <c r="E180">
+        <v>41</v>
+      </c>
+      <c r="H180" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="181" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A181" s="2">
+        <v>43918</v>
+      </c>
+      <c r="B181" t="s">
+        <v>11</v>
+      </c>
+      <c r="C181" t="s">
+        <v>29</v>
+      </c>
+      <c r="D181">
+        <f t="shared" si="0"/>
+        <v>1163</v>
+      </c>
+      <c r="E181">
+        <v>18</v>
+      </c>
+      <c r="H181" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="182" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A182" s="2">
+        <v>43918</v>
+      </c>
+      <c r="B182" t="s">
+        <v>10</v>
+      </c>
+      <c r="C182" t="s">
+        <v>29</v>
+      </c>
+      <c r="D182">
+        <f t="shared" si="0"/>
+        <v>1175</v>
+      </c>
+      <c r="E182">
+        <v>12</v>
+      </c>
+      <c r="H182" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="183" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A183" s="2">
+        <v>43918</v>
+      </c>
+      <c r="B183" t="s">
+        <v>8</v>
+      </c>
+      <c r="C183" t="s">
+        <v>28</v>
+      </c>
+      <c r="D183">
+        <f t="shared" si="0"/>
+        <v>1187</v>
+      </c>
+      <c r="E183">
+        <v>12</v>
+      </c>
+      <c r="H183" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="184" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A184" s="2">
+        <v>43918</v>
+      </c>
+      <c r="B184" t="s">
+        <v>18</v>
+      </c>
+      <c r="C184" t="s">
+        <v>18</v>
+      </c>
+      <c r="D184">
+        <f t="shared" si="0"/>
+        <v>1193</v>
+      </c>
+      <c r="E184">
+        <v>6</v>
+      </c>
+      <c r="H184" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="185" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A185" s="2">
+        <v>43918</v>
+      </c>
+      <c r="B185" t="s">
+        <v>31</v>
+      </c>
+      <c r="C185" t="s">
+        <v>31</v>
+      </c>
+      <c r="D185">
+        <f t="shared" si="0"/>
+        <v>1196</v>
+      </c>
+      <c r="E185">
+        <v>3</v>
+      </c>
+      <c r="H185" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="186" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A186" s="2">
+        <v>43918</v>
+      </c>
+      <c r="B186" t="s">
+        <v>73</v>
+      </c>
+      <c r="C186" t="s">
+        <v>30</v>
+      </c>
+      <c r="D186">
+        <f t="shared" si="0"/>
+        <v>1199</v>
+      </c>
+      <c r="E186">
+        <v>3</v>
+      </c>
+      <c r="H186" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="187" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A187" s="2">
+        <v>43918</v>
+      </c>
+      <c r="B187" t="s">
+        <v>65</v>
+      </c>
+      <c r="C187" t="s">
+        <v>30</v>
+      </c>
+      <c r="D187">
+        <f t="shared" si="0"/>
+        <v>1200</v>
+      </c>
+      <c r="E187">
+        <v>1</v>
+      </c>
+      <c r="H187" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="188" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A188" s="2">
+        <v>43918</v>
+      </c>
+      <c r="B188" t="s">
+        <v>12</v>
+      </c>
+      <c r="C188" t="s">
+        <v>28</v>
+      </c>
+      <c r="D188">
+        <f t="shared" si="0"/>
+        <v>1201</v>
+      </c>
+      <c r="E188">
+        <v>1</v>
+      </c>
+      <c r="H188" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="189" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A189" s="2">
+        <v>43918</v>
+      </c>
+      <c r="B189" t="s">
+        <v>13</v>
+      </c>
+      <c r="C189" t="s">
+        <v>28</v>
+      </c>
+      <c r="D189">
+        <f t="shared" si="0"/>
+        <v>1202</v>
+      </c>
+      <c r="E189">
+        <v>1</v>
+      </c>
+      <c r="H189" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="190" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A190" s="2">
+        <v>43918</v>
+      </c>
+      <c r="B190" t="s">
+        <v>8</v>
+      </c>
+      <c r="C190" t="s">
+        <v>28</v>
+      </c>
+      <c r="D190">
+        <f t="shared" si="0"/>
+        <v>1203</v>
+      </c>
+      <c r="E190">
+        <v>1</v>
+      </c>
+      <c r="H190" t="s">
         <v>59</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update dataset, update some visualizations
</commit_message>
<xml_diff>
--- a/data/corona_cases_ksa.xlsx
+++ b/data/corona_cases_ksa.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mohammedalawami/Desktop/Learn Data Science/Projects/corona-data-challenge/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62CEB2B6-07F9-1346-BFD6-26D65AB96BC5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C49CA15-BF86-4D40-875C-AF6F55658B8F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="33600" windowHeight="20640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="737" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="773" uniqueCount="75">
   <si>
     <t>date</t>
   </si>
@@ -252,6 +252,9 @@
   </si>
   <si>
     <t>Khamis Mushait</t>
+  </si>
+  <si>
+    <t>Ras Tanura</t>
   </si>
 </sst>
 </file>
@@ -666,10 +669,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N190"/>
+  <dimension ref="A1:N204"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A159" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="G192" sqref="G192"/>
+    <sheetView tabSelected="1" topLeftCell="A181" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A203" sqref="A203"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3356,7 +3359,7 @@
         <v>43910</v>
       </c>
       <c r="B109" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="C109" t="s">
         <v>31</v>
@@ -3926,7 +3929,7 @@
         <v>9</v>
       </c>
       <c r="D137">
-        <f t="shared" ref="D137:D190" si="0" xml:space="preserve"> D136+E137</f>
+        <f t="shared" ref="D137:D200" si="0" xml:space="preserve"> D136+E137</f>
         <v>713</v>
       </c>
       <c r="E137">
@@ -4893,10 +4896,10 @@
       </c>
       <c r="D183">
         <f t="shared" si="0"/>
-        <v>1187</v>
+        <v>1188</v>
       </c>
       <c r="E183">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H183" t="s">
         <v>59</v>
@@ -4914,7 +4917,7 @@
       </c>
       <c r="D184">
         <f t="shared" si="0"/>
-        <v>1193</v>
+        <v>1194</v>
       </c>
       <c r="E184">
         <v>6</v>
@@ -4935,7 +4938,7 @@
       </c>
       <c r="D185">
         <f t="shared" si="0"/>
-        <v>1196</v>
+        <v>1197</v>
       </c>
       <c r="E185">
         <v>3</v>
@@ -4956,7 +4959,7 @@
       </c>
       <c r="D186">
         <f t="shared" si="0"/>
-        <v>1199</v>
+        <v>1200</v>
       </c>
       <c r="E186">
         <v>3</v>
@@ -4977,7 +4980,7 @@
       </c>
       <c r="D187">
         <f t="shared" si="0"/>
-        <v>1200</v>
+        <v>1201</v>
       </c>
       <c r="E187">
         <v>1</v>
@@ -4998,7 +5001,7 @@
       </c>
       <c r="D188">
         <f t="shared" si="0"/>
-        <v>1201</v>
+        <v>1202</v>
       </c>
       <c r="E188">
         <v>1</v>
@@ -5019,7 +5022,7 @@
       </c>
       <c r="D189">
         <f t="shared" si="0"/>
-        <v>1202</v>
+        <v>1203</v>
       </c>
       <c r="E189">
         <v>1</v>
@@ -5030,24 +5033,279 @@
     </row>
     <row r="190" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A190" s="2">
-        <v>43918</v>
+        <v>43919</v>
       </c>
       <c r="B190" t="s">
+        <v>9</v>
+      </c>
+      <c r="C190" t="s">
+        <v>9</v>
+      </c>
+      <c r="D190">
+        <f t="shared" si="0"/>
+        <v>1230</v>
+      </c>
+      <c r="E190">
+        <v>27</v>
+      </c>
+      <c r="H190" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="191" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A191" s="2">
+        <v>43919</v>
+      </c>
+      <c r="B191" t="s">
+        <v>15</v>
+      </c>
+      <c r="C191" t="s">
+        <v>28</v>
+      </c>
+      <c r="D191">
+        <f t="shared" si="0"/>
+        <v>1244</v>
+      </c>
+      <c r="E191">
+        <v>14</v>
+      </c>
+      <c r="H191" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="192" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A192" s="2">
+        <v>43919</v>
+      </c>
+      <c r="B192" t="s">
+        <v>18</v>
+      </c>
+      <c r="C192" t="s">
+        <v>18</v>
+      </c>
+      <c r="D192">
+        <f t="shared" si="0"/>
+        <v>1267</v>
+      </c>
+      <c r="E192">
+        <v>23</v>
+      </c>
+      <c r="H192" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="193" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A193" s="2">
+        <v>43919</v>
+      </c>
+      <c r="B193" t="s">
+        <v>11</v>
+      </c>
+      <c r="C193" t="s">
+        <v>29</v>
+      </c>
+      <c r="D193">
+        <f t="shared" si="0"/>
+        <v>1279</v>
+      </c>
+      <c r="E193">
+        <v>12</v>
+      </c>
+      <c r="H193" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="194" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A194" s="2">
+        <v>43919</v>
+      </c>
+      <c r="B194" t="s">
+        <v>10</v>
+      </c>
+      <c r="C194" t="s">
+        <v>29</v>
+      </c>
+      <c r="D194">
+        <f t="shared" si="0"/>
+        <v>1286</v>
+      </c>
+      <c r="E194">
+        <v>7</v>
+      </c>
+      <c r="H194" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="195" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A195" s="2">
+        <v>43919</v>
+      </c>
+      <c r="B195" t="s">
+        <v>13</v>
+      </c>
+      <c r="C195" t="s">
+        <v>28</v>
+      </c>
+      <c r="D195">
+        <f t="shared" si="0"/>
+        <v>1290</v>
+      </c>
+      <c r="E195">
+        <v>4</v>
+      </c>
+      <c r="H195" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="196" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A196" s="2">
+        <v>43919</v>
+      </c>
+      <c r="B196" t="s">
+        <v>14</v>
+      </c>
+      <c r="C196" t="s">
+        <v>28</v>
+      </c>
+      <c r="D196">
+        <f t="shared" si="0"/>
+        <v>1292</v>
+      </c>
+      <c r="E196">
+        <v>2</v>
+      </c>
+      <c r="H196" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="197" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A197" s="2">
+        <v>43919</v>
+      </c>
+      <c r="B197" t="s">
         <v>8</v>
       </c>
-      <c r="C190" t="s">
-        <v>28</v>
-      </c>
-      <c r="D190">
-        <f t="shared" si="0"/>
-        <v>1203</v>
-      </c>
-      <c r="E190">
-        <v>1</v>
-      </c>
-      <c r="H190" t="s">
-        <v>59</v>
-      </c>
+      <c r="C197" t="s">
+        <v>28</v>
+      </c>
+      <c r="D197">
+        <f t="shared" si="0"/>
+        <v>1294</v>
+      </c>
+      <c r="E197">
+        <v>2</v>
+      </c>
+      <c r="H197" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="198" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A198" s="2">
+        <v>43919</v>
+      </c>
+      <c r="B198" t="s">
+        <v>74</v>
+      </c>
+      <c r="C198" t="s">
+        <v>28</v>
+      </c>
+      <c r="D198">
+        <f t="shared" si="0"/>
+        <v>1295</v>
+      </c>
+      <c r="E198">
+        <v>1</v>
+      </c>
+      <c r="H198" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="199" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A199" s="3">
+        <v>43919</v>
+      </c>
+      <c r="B199" t="s">
+        <v>25</v>
+      </c>
+      <c r="C199" t="s">
+        <v>29</v>
+      </c>
+      <c r="D199">
+        <f t="shared" si="0"/>
+        <v>1296</v>
+      </c>
+      <c r="E199">
+        <v>1</v>
+      </c>
+      <c r="H199" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="200" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A200" s="2">
+        <v>43919</v>
+      </c>
+      <c r="B200" t="s">
+        <v>12</v>
+      </c>
+      <c r="C200" t="s">
+        <v>28</v>
+      </c>
+      <c r="D200">
+        <f t="shared" si="0"/>
+        <v>1297</v>
+      </c>
+      <c r="E200">
+        <v>1</v>
+      </c>
+      <c r="H200" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="201" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A201" s="2">
+        <v>43919</v>
+      </c>
+      <c r="B201" t="s">
+        <v>73</v>
+      </c>
+      <c r="C201" t="s">
+        <v>30</v>
+      </c>
+      <c r="D201">
+        <f t="shared" ref="D201:D202" si="1" xml:space="preserve"> D200+E201</f>
+        <v>1298</v>
+      </c>
+      <c r="E201">
+        <v>1</v>
+      </c>
+      <c r="H201" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="202" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A202" s="2">
+        <v>43919</v>
+      </c>
+      <c r="B202" t="s">
+        <v>31</v>
+      </c>
+      <c r="C202" t="s">
+        <v>31</v>
+      </c>
+      <c r="D202">
+        <f t="shared" si="1"/>
+        <v>1299</v>
+      </c>
+      <c r="E202">
+        <v>1</v>
+      </c>
+      <c r="H202" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="204" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A204" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>